<commit_message>
HNI DEV | #4347 | All DS/My DS page: Validations are not retained properly
</commit_message>
<xml_diff>
--- a/datawinners/media/files/DataWinners_ImportDataSenders.xlsx
+++ b/datawinners/media/files/DataWinners_ImportDataSenders.xlsx
@@ -236,7 +236,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -266,12 +266,6 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -291,7 +285,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -319,20 +313,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="55"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -349,10 +334,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,11 +784,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -839,13 +821,6 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -869,25 +844,25 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="8" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>